<commit_message>
EPBDS: Added java comments to source and updated unit tests.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
@@ -97,12 +97,6 @@
     <t>Datatype State1 &lt;String&gt;</t>
   </si>
   <si>
-    <t>//Datatype State2 &lt;String&gt;</t>
-  </si>
-  <si>
-    <t>//Datatype MyInt3 &lt;int&gt;</t>
-  </si>
-  <si>
     <t>MyRange x = new IntRange("1 .. 100");
 IntRange y = x; 
 MyBool result = y.contains(z);
@@ -148,9 +142,6 @@
     <t>6 - 9</t>
   </si>
   <si>
-    <t>Rules int testStringAliasType(State1 state)</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -167,6 +158,15 @@
   </si>
   <si>
     <t>Rules int testIntRangeAliasType2(int i)</t>
+  </si>
+  <si>
+    <t>Datatype MyInt3 &lt;int&gt;</t>
+  </si>
+  <si>
+    <t>Datatype State3 &lt;String&gt;</t>
+  </si>
+  <si>
+    <t>Rules int testStringAliasType(State3 state)</t>
   </si>
 </sst>
 </file>
@@ -423,6 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -430,6 +431,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -441,19 +451,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E44" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -792,27 +792,27 @@
     </row>
     <row r="8" spans="2:2">
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:2">
@@ -820,7 +820,7 @@
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:5">
@@ -859,7 +859,7 @@
         <v>15</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="2:5">
@@ -867,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:5">
@@ -881,18 +881,18 @@
     <row r="31" spans="2:5">
       <c r="B31" s="5"/>
       <c r="E31" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="5"/>
       <c r="E32" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="E33" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -911,11 +911,11 @@
       </c>
     </row>
     <row r="42" spans="2:5">
-      <c r="B42" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="11"/>
+      <c r="B42" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="4" t="s">
@@ -929,10 +929,10 @@
       </c>
     </row>
     <row r="50" spans="2:3">
-      <c r="B50" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C50" s="11"/>
+      <c r="B50" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="12"/>
     </row>
     <row r="51" spans="2:3">
       <c r="B51" s="6">
@@ -957,7 +957,7 @@
   <dimension ref="B3:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F3" sqref="F3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -971,14 +971,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="F3" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="F3" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1" t="s">
@@ -1000,13 +1000,13 @@
       </c>
       <c r="C5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -1073,14 +1073,14 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="F13" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="F13" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="1" t="s">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="C15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1175,14 +1175,14 @@
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="F23" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="F23" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="1" t="s">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1216,7 +1216,7 @@
         <v>8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>8</v>
@@ -1243,7 +1243,7 @@
       <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G28" s="1">
@@ -1259,46 +1259,46 @@
       </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="18"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
     </row>
     <row r="32" spans="2:7" ht="32.25" customHeight="1">
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="15"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="19"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
+      <c r="B34" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
     </row>
     <row r="35" spans="2:4" ht="32.25" customHeight="1">
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="19"/>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="18"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="16"/>
     </row>
     <row r="38" spans="2:4" ht="69.75" customHeight="1">
-      <c r="B38" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="15"/>
+      <c r="B38" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
EPBDS: fixed the following bug: invalid value of domain type is loaded successfully in testmethod table component.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
@@ -433,6 +433,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -450,9 +453,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -957,7 +957,7 @@
   <dimension ref="B3:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G3"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -971,14 +971,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="F3" s="20" t="s">
+      <c r="C3" s="14"/>
+      <c r="F3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1" t="s">
@@ -1073,14 +1073,14 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="F13" s="20" t="s">
+      <c r="C13" s="14"/>
+      <c r="F13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="20"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="1" t="s">
@@ -1167,22 +1167,24 @@
       <c r="C20" s="1">
         <v>1</v>
       </c>
-      <c r="F20" s="1">
-        <v>3</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="F22" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="F23" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" s="12"/>
+      <c r="F23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="1" t="s">
@@ -1192,11 +1194,9 @@
         <v>6</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="1" t="s">
@@ -1204,9 +1204,11 @@
       </c>
       <c r="C25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" s="1" t="s">
@@ -1216,10 +1218,10 @@
         <v>8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:7">
@@ -1229,11 +1231,11 @@
       <c r="C27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>9</v>
+      <c r="F27" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7">
@@ -1243,70 +1245,59 @@
       <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="F28" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="1">
-        <v>1</v>
+      <c r="G28" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:7">
       <c r="C29" s="8">
         <v>0</v>
       </c>
-      <c r="G29" s="8">
-        <v>0</v>
-      </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" spans="2:7" ht="32.25" customHeight="1">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
     </row>
     <row r="35" spans="2:4" ht="32.25" customHeight="1">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="17"/>
     </row>
     <row r="38" spans="2:4" ht="69.75" customHeight="1">
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B3:C3"/>
@@ -1314,6 +1305,11 @@
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-1509 Added check of input parameters to method invocation mechanism: if input parameter and appropriate method parameter has different types (used in case of alias types) then cast types before method invocation.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="21855" windowHeight="10680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="21855" windowHeight="10680"/>
   </bookViews>
   <sheets>
     <sheet name="Alias Datatype Declaration" sheetId="1" r:id="rId1"/>
@@ -433,9 +433,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,6 +450,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -971,14 +971,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="C3" s="20"/>
+      <c r="F3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="14"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1" t="s">
@@ -1073,14 +1073,14 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="F13" s="14" t="s">
+      <c r="C13" s="20"/>
+      <c r="F13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="14"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="1" t="s">
@@ -1250,54 +1250,62 @@
       </c>
     </row>
     <row r="29" spans="2:7">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
       <c r="C29" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="17"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
     </row>
     <row r="32" spans="2:7" ht="32.25" customHeight="1">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="19"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="17"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
     </row>
     <row r="35" spans="2:4" ht="32.25" customHeight="1">
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="19"/>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="17"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="16"/>
     </row>
     <row r="38" spans="2:4" ht="69.75" customHeight="1">
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B3:C3"/>
@@ -1305,11 +1313,6 @@
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-2028 Fixed bug. Test.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="21855" windowHeight="10680"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="21855" windowHeight="10680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Alias Datatype Declaration" sheetId="1" r:id="rId1"/>
     <sheet name="Alias Datatype Usage Proper" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>CA</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>Rules int testStringAliasType(State3 state)</t>
+  </si>
+  <si>
+    <t>Rules int testAliasTypeAsArrays(State3 state)</t>
+  </si>
+  <si>
+    <t>State3[]</t>
+  </si>
+  <si>
+    <t>CA,AR</t>
   </si>
 </sst>
 </file>
@@ -433,6 +442,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -450,9 +462,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -954,10 +963,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:G38"/>
+  <dimension ref="B3:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -970,17 +979,21 @@
     <col min="11" max="11" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="2:11">
+      <c r="B3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="F3" s="20" t="s">
+      <c r="C3" s="14"/>
+      <c r="F3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="20"/>
-    </row>
-    <row r="4" spans="2:7">
+      <c r="G3" s="14"/>
+      <c r="J3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" spans="2:11">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -993,8 +1006,14 @@
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="2:7">
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1003,8 +1022,12 @@
         <v>40</v>
       </c>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="2:7">
+      <c r="J5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="2:11">
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1015,8 +1038,14 @@
       <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:7">
+      <c r="J6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1029,8 +1058,14 @@
       <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:7">
+      <c r="J7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,8 +1078,14 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="J8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1057,8 +1098,14 @@
       <c r="G9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:7">
+      <c r="J9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1072,17 +1119,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="20" t="s">
+    <row r="13" spans="2:11">
+      <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="F13" s="20" t="s">
+      <c r="C13" s="14"/>
+      <c r="F13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="20"/>
-    </row>
-    <row r="14" spans="2:7">
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="2:11">
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1096,7 +1143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:11">
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1106,7 +1153,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="2:7">
+    <row r="16" spans="2:11">
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1258,54 +1305,50 @@
       </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" spans="2:7" ht="32.25" customHeight="1">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
     </row>
     <row r="35" spans="2:4" ht="32.25" customHeight="1">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="17"/>
     </row>
     <row r="38" spans="2:4" ht="69.75" customHeight="1">
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
+  <mergeCells count="13">
+    <mergeCell ref="J3:K3"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B3:C3"/>
@@ -1313,6 +1356,11 @@
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>